<commit_message>
Query vaues from output excel to sql database
</commit_message>
<xml_diff>
--- a/protocol/output.xlsx
+++ b/protocol/output.xlsx
@@ -575,7 +575,7 @@
         <v>Longitudinal</v>
       </c>
       <c r="C9" t="str">
-        <v>P2</v>
+        <v>2</v>
       </c>
       <c r="D9" t="str">
         <v>4</v>
@@ -601,7 +601,7 @@
         <v>Longitudinal</v>
       </c>
       <c r="C10" t="str">
-        <v>P2</v>
+        <v>2</v>
       </c>
       <c r="D10" t="str">
         <v>4</v>
@@ -627,7 +627,7 @@
         <v>Longitudinal</v>
       </c>
       <c r="C11" t="str">
-        <v>P2</v>
+        <v>2</v>
       </c>
       <c r="D11" t="str">
         <v>4</v>
@@ -653,7 +653,7 @@
         <v>Longitudinal</v>
       </c>
       <c r="C12" t="str">
-        <v>P2</v>
+        <v>2</v>
       </c>
       <c r="D12" t="str">
         <v>4</v>
@@ -679,7 +679,7 @@
         <v>Longitudinal</v>
       </c>
       <c r="C13" t="str">
-        <v>P2</v>
+        <v>2</v>
       </c>
       <c r="D13" t="str">
         <v>4</v>
@@ -705,7 +705,7 @@
         <v>Longitudinal</v>
       </c>
       <c r="C14" t="str">
-        <v>P2</v>
+        <v>2</v>
       </c>
       <c r="D14" t="str">
         <v>4</v>
@@ -731,7 +731,7 @@
         <v>Longitudinal</v>
       </c>
       <c r="C15" t="str">
-        <v>P2</v>
+        <v>2</v>
       </c>
       <c r="D15" t="str">
         <v>5</v>
@@ -757,7 +757,7 @@
         <v>Longitudinal</v>
       </c>
       <c r="C16" t="str">
-        <v>P2</v>
+        <v>2</v>
       </c>
       <c r="D16" t="str">
         <v>5</v>
@@ -783,7 +783,7 @@
         <v>Longitudinal</v>
       </c>
       <c r="C17" t="str">
-        <v>P2</v>
+        <v>2</v>
       </c>
       <c r="D17" t="str">
         <v>5</v>
@@ -809,7 +809,7 @@
         <v>Longitudinal</v>
       </c>
       <c r="C18" t="str">
-        <v>P2</v>
+        <v>2</v>
       </c>
       <c r="D18" t="str">
         <v>5</v>
@@ -835,7 +835,7 @@
         <v>Longitudinal</v>
       </c>
       <c r="C19" t="str">
-        <v>P2</v>
+        <v>2</v>
       </c>
       <c r="D19" t="str">
         <v>5</v>
@@ -861,7 +861,7 @@
         <v>Longitudinal</v>
       </c>
       <c r="C20" t="str">
-        <v>P2</v>
+        <v>2</v>
       </c>
       <c r="D20" t="str">
         <v>5</v>
@@ -887,7 +887,7 @@
         <v>Longitudinal</v>
       </c>
       <c r="C21" t="str">
-        <v>P2</v>
+        <v>2</v>
       </c>
       <c r="D21" t="str">
         <v>L3</v>
@@ -913,7 +913,7 @@
         <v>Longitudinal</v>
       </c>
       <c r="C22" t="str">
-        <v>P2</v>
+        <v>2</v>
       </c>
       <c r="D22" t="str">
         <v>L3</v>
@@ -939,7 +939,7 @@
         <v>Longitudinal</v>
       </c>
       <c r="C23" t="str">
-        <v>P2</v>
+        <v>2</v>
       </c>
       <c r="D23" t="str">
         <v>L3</v>
@@ -965,7 +965,7 @@
         <v>Longitudinal</v>
       </c>
       <c r="C24" t="str">
-        <v>P2</v>
+        <v>2</v>
       </c>
       <c r="D24" t="str">
         <v>L3</v>
@@ -991,7 +991,7 @@
         <v>Longitudinal</v>
       </c>
       <c r="C25" t="str">
-        <v>P2</v>
+        <v>2</v>
       </c>
       <c r="D25" t="str">
         <v>L3</v>
@@ -1017,7 +1017,7 @@
         <v>Longitudinal</v>
       </c>
       <c r="C26" t="str">
-        <v>P2</v>
+        <v>2</v>
       </c>
       <c r="D26" t="str">
         <v>L3</v>
@@ -1355,7 +1355,7 @@
         <v>Lateral</v>
       </c>
       <c r="C39" t="str">
-        <v>P2</v>
+        <v>2</v>
       </c>
       <c r="D39" t="str">
         <v>4</v>
@@ -1381,7 +1381,7 @@
         <v>Lateral</v>
       </c>
       <c r="C40" t="str">
-        <v>P2</v>
+        <v>2</v>
       </c>
       <c r="D40" t="str">
         <v>4</v>
@@ -1407,7 +1407,7 @@
         <v>Lateral</v>
       </c>
       <c r="C41" t="str">
-        <v>P2</v>
+        <v>2</v>
       </c>
       <c r="D41" t="str">
         <v>4</v>
@@ -1433,7 +1433,7 @@
         <v>Lateral</v>
       </c>
       <c r="C42" t="str">
-        <v>P2</v>
+        <v>2</v>
       </c>
       <c r="D42" t="str">
         <v>4</v>
@@ -1459,7 +1459,7 @@
         <v>Lateral</v>
       </c>
       <c r="C43" t="str">
-        <v>P2</v>
+        <v>2</v>
       </c>
       <c r="D43" t="str">
         <v>4</v>
@@ -1485,7 +1485,7 @@
         <v>Lateral</v>
       </c>
       <c r="C44" t="str">
-        <v>P2</v>
+        <v>2</v>
       </c>
       <c r="D44" t="str">
         <v>4</v>
@@ -1511,7 +1511,7 @@
         <v>Lateral</v>
       </c>
       <c r="C45" t="str">
-        <v>P2</v>
+        <v>2</v>
       </c>
       <c r="D45" t="str">
         <v>5</v>
@@ -1537,7 +1537,7 @@
         <v>Lateral</v>
       </c>
       <c r="C46" t="str">
-        <v>P2</v>
+        <v>2</v>
       </c>
       <c r="D46" t="str">
         <v>5</v>
@@ -1563,7 +1563,7 @@
         <v>Lateral</v>
       </c>
       <c r="C47" t="str">
-        <v>P2</v>
+        <v>2</v>
       </c>
       <c r="D47" t="str">
         <v>5</v>
@@ -1589,7 +1589,7 @@
         <v>Lateral</v>
       </c>
       <c r="C48" t="str">
-        <v>P2</v>
+        <v>2</v>
       </c>
       <c r="D48" t="str">
         <v>5</v>
@@ -1615,7 +1615,7 @@
         <v>Lateral</v>
       </c>
       <c r="C49" t="str">
-        <v>P2</v>
+        <v>2</v>
       </c>
       <c r="D49" t="str">
         <v>5</v>
@@ -1641,7 +1641,7 @@
         <v>Lateral</v>
       </c>
       <c r="C50" t="str">
-        <v>P2</v>
+        <v>2</v>
       </c>
       <c r="D50" t="str">
         <v>5</v>
@@ -1667,7 +1667,7 @@
         <v>Lateral</v>
       </c>
       <c r="C51" t="str">
-        <v>P2</v>
+        <v>2</v>
       </c>
       <c r="D51" t="str">
         <v>L3</v>
@@ -1693,7 +1693,7 @@
         <v>Lateral</v>
       </c>
       <c r="C52" t="str">
-        <v>P2</v>
+        <v>2</v>
       </c>
       <c r="D52" t="str">
         <v>L3</v>
@@ -1719,7 +1719,7 @@
         <v>Lateral</v>
       </c>
       <c r="C53" t="str">
-        <v>P2</v>
+        <v>2</v>
       </c>
       <c r="D53" t="str">
         <v>L3</v>
@@ -1745,7 +1745,7 @@
         <v>Lateral</v>
       </c>
       <c r="C54" t="str">
-        <v>P2</v>
+        <v>2</v>
       </c>
       <c r="D54" t="str">
         <v>L3</v>
@@ -1771,7 +1771,7 @@
         <v>Lateral</v>
       </c>
       <c r="C55" t="str">
-        <v>P2</v>
+        <v>2</v>
       </c>
       <c r="D55" t="str">
         <v>L3</v>
@@ -1797,7 +1797,7 @@
         <v>Lateral</v>
       </c>
       <c r="C56" t="str">
-        <v>P2</v>
+        <v>2</v>
       </c>
       <c r="D56" t="str">
         <v>L3</v>
@@ -1979,7 +1979,7 @@
         <v>Combined</v>
       </c>
       <c r="C63" t="str">
-        <v>P2</v>
+        <v>2</v>
       </c>
       <c r="D63" t="str">
         <v>4,5,L3</v>
@@ -2005,7 +2005,7 @@
         <v>Combined</v>
       </c>
       <c r="C64" t="str">
-        <v>P2</v>
+        <v>2</v>
       </c>
       <c r="D64" t="str">
         <v>4,5,L3</v>
@@ -2031,7 +2031,7 @@
         <v>Combined</v>
       </c>
       <c r="C65" t="str">
-        <v>P2</v>
+        <v>2</v>
       </c>
       <c r="D65" t="str">
         <v>4,5,L3</v>
@@ -2057,7 +2057,7 @@
         <v>Combined</v>
       </c>
       <c r="C66" t="str">
-        <v>P2</v>
+        <v>2</v>
       </c>
       <c r="D66" t="str">
         <v>4,5,L3</v>
@@ -2083,7 +2083,7 @@
         <v>Combined</v>
       </c>
       <c r="C67" t="str">
-        <v>P2</v>
+        <v>2</v>
       </c>
       <c r="D67" t="str">
         <v>4,5,L3</v>
@@ -2109,7 +2109,7 @@
         <v>Combined</v>
       </c>
       <c r="C68" t="str">
-        <v>P2</v>
+        <v>2</v>
       </c>
       <c r="D68" t="str">
         <v>4,5,L3</v>
@@ -2135,7 +2135,7 @@
         <v>Combined</v>
       </c>
       <c r="C69" t="str">
-        <v>P2</v>
+        <v>2</v>
       </c>
       <c r="D69" t="str">
         <v>4,5,L3</v>
@@ -2161,7 +2161,7 @@
         <v>Combined</v>
       </c>
       <c r="C70" t="str">
-        <v>P2</v>
+        <v>2</v>
       </c>
       <c r="D70" t="str">
         <v>4,5,L3</v>
@@ -2187,7 +2187,7 @@
         <v>Combined</v>
       </c>
       <c r="C71" t="str">
-        <v>P2</v>
+        <v>2</v>
       </c>
       <c r="D71" t="str">
         <v>4,5,L3</v>
@@ -2213,7 +2213,7 @@
         <v>Combined</v>
       </c>
       <c r="C72" t="str">
-        <v>P2</v>
+        <v>2</v>
       </c>
       <c r="D72" t="str">
         <v>4,5,L3</v>
@@ -2239,7 +2239,7 @@
         <v>Combined</v>
       </c>
       <c r="C73" t="str">
-        <v>P2</v>
+        <v>2</v>
       </c>
       <c r="D73" t="str">
         <v>4,5,L3</v>
@@ -2265,7 +2265,7 @@
         <v>Combined</v>
       </c>
       <c r="C74" t="str">
-        <v>P2</v>
+        <v>2</v>
       </c>
       <c r="D74" t="str">
         <v>4,5,L3</v>
@@ -2291,7 +2291,7 @@
         <v>Combined</v>
       </c>
       <c r="C75" t="str">
-        <v>P2</v>
+        <v>2</v>
       </c>
       <c r="D75" t="str">
         <v>4,5,L3</v>
@@ -2317,7 +2317,7 @@
         <v>Combined</v>
       </c>
       <c r="C76" t="str">
-        <v>P2</v>
+        <v>2</v>
       </c>
       <c r="D76" t="str">
         <v>4,5,L3</v>
@@ -2343,7 +2343,7 @@
         <v>Combined</v>
       </c>
       <c r="C77" t="str">
-        <v>P2</v>
+        <v>2</v>
       </c>
       <c r="D77" t="str">
         <v>4,5,L3</v>
@@ -2369,7 +2369,7 @@
         <v>Combined</v>
       </c>
       <c r="C78" t="str">
-        <v>P2</v>
+        <v>2</v>
       </c>
       <c r="D78" t="str">
         <v>4,5,L3</v>
@@ -2395,7 +2395,7 @@
         <v>Combined</v>
       </c>
       <c r="C79" t="str">
-        <v>P2</v>
+        <v>2</v>
       </c>
       <c r="D79" t="str">
         <v>4,5,L3</v>
@@ -2421,7 +2421,7 @@
         <v>Combined</v>
       </c>
       <c r="C80" t="str">
-        <v>P2</v>
+        <v>2</v>
       </c>
       <c r="D80" t="str">
         <v>4,5,L3</v>
@@ -2447,7 +2447,7 @@
         <v>Combined</v>
       </c>
       <c r="C81" t="str">
-        <v>P2</v>
+        <v>2</v>
       </c>
       <c r="D81" t="str">
         <v>4,5,L3</v>
@@ -2473,7 +2473,7 @@
         <v>Combined</v>
       </c>
       <c r="C82" t="str">
-        <v>P2</v>
+        <v>2</v>
       </c>
       <c r="D82" t="str">
         <v>4,5,L3</v>
@@ -2499,7 +2499,7 @@
         <v>Combined</v>
       </c>
       <c r="C83" t="str">
-        <v>P2</v>
+        <v>2</v>
       </c>
       <c r="D83" t="str">
         <v>4,5,L3</v>
@@ -2525,7 +2525,7 @@
         <v>Combined</v>
       </c>
       <c r="C84" t="str">
-        <v>P2</v>
+        <v>2</v>
       </c>
       <c r="D84" t="str">
         <v>4,5,L3</v>
@@ -2551,7 +2551,7 @@
         <v>Combined</v>
       </c>
       <c r="C85" t="str">
-        <v>P2</v>
+        <v>2</v>
       </c>
       <c r="D85" t="str">
         <v>4,5,L3</v>
@@ -2577,7 +2577,7 @@
         <v>Combined</v>
       </c>
       <c r="C86" t="str">
-        <v>P2</v>
+        <v>2</v>
       </c>
       <c r="D86" t="str">
         <v>4,5,L3</v>
@@ -2993,7 +2993,7 @@
         <v>Loaded Radius &amp; Rolling Radius</v>
       </c>
       <c r="C102" t="str">
-        <v>P2</v>
+        <v>2</v>
       </c>
       <c r="D102" t="str">
         <v>4</v>
@@ -3019,7 +3019,7 @@
         <v>Loaded Radius &amp; Rolling Radius</v>
       </c>
       <c r="C103" t="str">
-        <v>P2</v>
+        <v>2</v>
       </c>
       <c r="D103" t="str">
         <v>4</v>
@@ -3045,7 +3045,7 @@
         <v>Loaded Radius &amp; Rolling Radius</v>
       </c>
       <c r="C104" t="str">
-        <v>P2</v>
+        <v>2</v>
       </c>
       <c r="D104" t="str">
         <v>4</v>
@@ -3071,7 +3071,7 @@
         <v>Loaded Radius &amp; Rolling Radius</v>
       </c>
       <c r="C105" t="str">
-        <v>P2</v>
+        <v>2</v>
       </c>
       <c r="D105" t="str">
         <v>4</v>
@@ -3097,7 +3097,7 @@
         <v>Loaded Radius &amp; Rolling Radius</v>
       </c>
       <c r="C106" t="str">
-        <v>P2</v>
+        <v>2</v>
       </c>
       <c r="D106" t="str">
         <v>4</v>
@@ -3123,7 +3123,7 @@
         <v>Loaded Radius &amp; Rolling Radius</v>
       </c>
       <c r="C107" t="str">
-        <v>P2</v>
+        <v>2</v>
       </c>
       <c r="D107" t="str">
         <v>5</v>
@@ -3149,7 +3149,7 @@
         <v>Loaded Radius &amp; Rolling Radius</v>
       </c>
       <c r="C108" t="str">
-        <v>P2</v>
+        <v>2</v>
       </c>
       <c r="D108" t="str">
         <v>5</v>
@@ -3175,7 +3175,7 @@
         <v>Loaded Radius &amp; Rolling Radius</v>
       </c>
       <c r="C109" t="str">
-        <v>P2</v>
+        <v>2</v>
       </c>
       <c r="D109" t="str">
         <v>5</v>
@@ -3201,7 +3201,7 @@
         <v>Loaded Radius &amp; Rolling Radius</v>
       </c>
       <c r="C110" t="str">
-        <v>P2</v>
+        <v>2</v>
       </c>
       <c r="D110" t="str">
         <v>5</v>
@@ -3227,7 +3227,7 @@
         <v>Loaded Radius &amp; Rolling Radius</v>
       </c>
       <c r="C111" t="str">
-        <v>P2</v>
+        <v>2</v>
       </c>
       <c r="D111" t="str">
         <v>5</v>
@@ -3253,7 +3253,7 @@
         <v>Loaded Radius &amp; Rolling Radius</v>
       </c>
       <c r="C112" t="str">
-        <v>P2</v>
+        <v>2</v>
       </c>
       <c r="D112" t="str">
         <v>L3</v>
@@ -3279,7 +3279,7 @@
         <v>Loaded Radius &amp; Rolling Radius</v>
       </c>
       <c r="C113" t="str">
-        <v>P2</v>
+        <v>2</v>
       </c>
       <c r="D113" t="str">
         <v>L3</v>
@@ -3305,7 +3305,7 @@
         <v>Loaded Radius &amp; Rolling Radius</v>
       </c>
       <c r="C114" t="str">
-        <v>P2</v>
+        <v>2</v>
       </c>
       <c r="D114" t="str">
         <v>L3</v>
@@ -3331,7 +3331,7 @@
         <v>Loaded Radius &amp; Rolling Radius</v>
       </c>
       <c r="C115" t="str">
-        <v>P2</v>
+        <v>2</v>
       </c>
       <c r="D115" t="str">
         <v>L3</v>
@@ -3357,7 +3357,7 @@
         <v>Loaded Radius &amp; Rolling Radius</v>
       </c>
       <c r="C116" t="str">
-        <v>P2</v>
+        <v>2</v>
       </c>
       <c r="D116" t="str">
         <v>L3</v>
@@ -3773,7 +3773,7 @@
         <v>Contact Patch Dimension</v>
       </c>
       <c r="C132" t="str">
-        <v>P2</v>
+        <v>2</v>
       </c>
       <c r="D132" t="str">
         <v>4</v>
@@ -3799,7 +3799,7 @@
         <v>Contact Patch Dimension</v>
       </c>
       <c r="C133" t="str">
-        <v>P2</v>
+        <v>2</v>
       </c>
       <c r="D133" t="str">
         <v>5</v>
@@ -3825,7 +3825,7 @@
         <v>Contact Patch Dimension</v>
       </c>
       <c r="C134" t="str">
-        <v>P2</v>
+        <v>2</v>
       </c>
       <c r="D134" t="str">
         <v>L3</v>
@@ -3929,7 +3929,7 @@
         <v>Longitudinal Transient Behaviour</v>
       </c>
       <c r="C138" t="str">
-        <v>P2</v>
+        <v>2</v>
       </c>
       <c r="D138" t="str">
         <v>4</v>
@@ -3955,7 +3955,7 @@
         <v>Longitudinal Transient Behaviour</v>
       </c>
       <c r="C139" t="str">
-        <v>P2</v>
+        <v>2</v>
       </c>
       <c r="D139" t="str">
         <v>5</v>
@@ -3981,7 +3981,7 @@
         <v>Longitudinal Transient Behaviour</v>
       </c>
       <c r="C140" t="str">
-        <v>P2</v>
+        <v>2</v>
       </c>
       <c r="D140" t="str">
         <v>L3</v>
@@ -4163,7 +4163,7 @@
         <v>Lateral Transient Behaviour</v>
       </c>
       <c r="C147" t="str">
-        <v>P2</v>
+        <v>2</v>
       </c>
       <c r="D147" t="str">
         <v>4</v>
@@ -4189,7 +4189,7 @@
         <v>Lateral Transient Behaviour</v>
       </c>
       <c r="C148" t="str">
-        <v>P2</v>
+        <v>2</v>
       </c>
       <c r="D148" t="str">
         <v>5</v>
@@ -4215,7 +4215,7 @@
         <v>Lateral Transient Behaviour</v>
       </c>
       <c r="C149" t="str">
-        <v>P2</v>
+        <v>2</v>
       </c>
       <c r="D149" t="str">
         <v>L3</v>
@@ -4371,7 +4371,7 @@
         <v>Yaw Stiffness</v>
       </c>
       <c r="C155" t="str">
-        <v>P2</v>
+        <v>2</v>
       </c>
       <c r="D155" t="str">
         <v>5</v>
@@ -4397,7 +4397,7 @@
         <v>Yaw Stiffness</v>
       </c>
       <c r="C156" t="str">
-        <v>P2</v>
+        <v>2</v>
       </c>
       <c r="D156" t="str">
         <v>5</v>
@@ -4724,7 +4724,7 @@
         <v>0  (Free Rolling)</v>
       </c>
       <c r="H168" t="str">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="169">
@@ -4750,7 +4750,7 @@
         <v>0  (Free Rolling)</v>
       </c>
       <c r="H169" t="str">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="170">
@@ -4776,7 +4776,7 @@
         <v>0  (Free Rolling)</v>
       </c>
       <c r="H170" t="str">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="171">
@@ -4787,7 +4787,7 @@
         <v>Rolling Resistance</v>
       </c>
       <c r="C171" t="str">
-        <v>P2</v>
+        <v>2</v>
       </c>
       <c r="D171" t="str">
         <v>4</v>
@@ -4813,7 +4813,7 @@
         <v>Rolling Resistance</v>
       </c>
       <c r="C172" t="str">
-        <v>P2</v>
+        <v>2</v>
       </c>
       <c r="D172" t="str">
         <v>5</v>
@@ -4839,7 +4839,7 @@
         <v>Rolling Resistance</v>
       </c>
       <c r="C173" t="str">
-        <v>P2</v>
+        <v>2</v>
       </c>
       <c r="D173" t="str">
         <v>L3</v>
@@ -4865,7 +4865,7 @@
         <v>Rolling Resistance</v>
       </c>
       <c r="C174" t="str">
-        <v>P2</v>
+        <v>2</v>
       </c>
       <c r="D174" t="str">
         <v>4</v>
@@ -4891,7 +4891,7 @@
         <v>Rolling Resistance</v>
       </c>
       <c r="C175" t="str">
-        <v>P2</v>
+        <v>2</v>
       </c>
       <c r="D175" t="str">
         <v>5</v>
@@ -4917,7 +4917,7 @@
         <v>Rolling Resistance</v>
       </c>
       <c r="C176" t="str">
-        <v>P2</v>
+        <v>2</v>
       </c>
       <c r="D176" t="str">
         <v>L3</v>
@@ -4943,7 +4943,7 @@
         <v>Rolling Resistance</v>
       </c>
       <c r="C177" t="str">
-        <v>P2</v>
+        <v>2</v>
       </c>
       <c r="D177" t="str">
         <v>4</v>
@@ -4969,7 +4969,7 @@
         <v>Rolling Resistance</v>
       </c>
       <c r="C178" t="str">
-        <v>P2</v>
+        <v>2</v>
       </c>
       <c r="D178" t="str">
         <v>5</v>
@@ -4995,7 +4995,7 @@
         <v>Rolling Resistance</v>
       </c>
       <c r="C179" t="str">
-        <v>P2</v>
+        <v>2</v>
       </c>
       <c r="D179" t="str">
         <v>L3</v>
@@ -5021,7 +5021,7 @@
         <v>Rolling Resistance</v>
       </c>
       <c r="C180" t="str">
-        <v>P2</v>
+        <v>2</v>
       </c>
       <c r="D180" t="str">
         <v>4</v>
@@ -5036,7 +5036,7 @@
         <v>0  (Free Rolling)</v>
       </c>
       <c r="H180" t="str">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="181">
@@ -5047,7 +5047,7 @@
         <v>Rolling Resistance</v>
       </c>
       <c r="C181" t="str">
-        <v>P2</v>
+        <v>2</v>
       </c>
       <c r="D181" t="str">
         <v>5</v>
@@ -5062,7 +5062,7 @@
         <v>0  (Free Rolling)</v>
       </c>
       <c r="H181" t="str">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="182">
@@ -5073,7 +5073,7 @@
         <v>Rolling Resistance</v>
       </c>
       <c r="C182" t="str">
-        <v>P2</v>
+        <v>2</v>
       </c>
       <c r="D182" t="str">
         <v>L3</v>
@@ -5088,7 +5088,7 @@
         <v>0  (Free Rolling)</v>
       </c>
       <c r="H182" t="str">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="183">
@@ -5348,7 +5348,7 @@
         <v>0  (Free Rolling)</v>
       </c>
       <c r="H192" t="str">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="193">
@@ -5374,7 +5374,7 @@
         <v>0  (Free Rolling)</v>
       </c>
       <c r="H193" t="str">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="194">
@@ -5400,7 +5400,7 @@
         <v>0  (Free Rolling)</v>
       </c>
       <c r="H194" t="str">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
display table in select.html, select.css and select.js
</commit_message>
<xml_diff>
--- a/protocol/output.xlsx
+++ b/protocol/output.xlsx
@@ -4646,7 +4646,7 @@
         <v>0  (Free Rolling)</v>
       </c>
       <c r="H165" t="str">
-        <v>V3</v>
+        <v>9</v>
       </c>
     </row>
     <row r="166">
@@ -4672,7 +4672,7 @@
         <v>0  (Free Rolling)</v>
       </c>
       <c r="H166" t="str">
-        <v>V3</v>
+        <v>9</v>
       </c>
     </row>
     <row r="167">
@@ -4698,7 +4698,7 @@
         <v>0  (Free Rolling)</v>
       </c>
       <c r="H167" t="str">
-        <v>V3</v>
+        <v>9</v>
       </c>
     </row>
     <row r="168">
@@ -4724,7 +4724,7 @@
         <v>0  (Free Rolling)</v>
       </c>
       <c r="H168" t="str">
-        <v>9</v>
+        <v>V4</v>
       </c>
     </row>
     <row r="169">
@@ -4750,7 +4750,7 @@
         <v>0  (Free Rolling)</v>
       </c>
       <c r="H169" t="str">
-        <v>9</v>
+        <v>V4</v>
       </c>
     </row>
     <row r="170">
@@ -4776,7 +4776,7 @@
         <v>0  (Free Rolling)</v>
       </c>
       <c r="H170" t="str">
-        <v>9</v>
+        <v>V4</v>
       </c>
     </row>
     <row r="171">
@@ -4958,7 +4958,7 @@
         <v>0  (Free Rolling)</v>
       </c>
       <c r="H177" t="str">
-        <v>V3</v>
+        <v>9</v>
       </c>
     </row>
     <row r="178">
@@ -4984,7 +4984,7 @@
         <v>0  (Free Rolling)</v>
       </c>
       <c r="H178" t="str">
-        <v>V3</v>
+        <v>9</v>
       </c>
     </row>
     <row r="179">
@@ -5010,7 +5010,7 @@
         <v>0  (Free Rolling)</v>
       </c>
       <c r="H179" t="str">
-        <v>V3</v>
+        <v>9</v>
       </c>
     </row>
     <row r="180">
@@ -5036,7 +5036,7 @@
         <v>0  (Free Rolling)</v>
       </c>
       <c r="H180" t="str">
-        <v>9</v>
+        <v>V4</v>
       </c>
     </row>
     <row r="181">
@@ -5062,7 +5062,7 @@
         <v>0  (Free Rolling)</v>
       </c>
       <c r="H181" t="str">
-        <v>9</v>
+        <v>V4</v>
       </c>
     </row>
     <row r="182">
@@ -5088,7 +5088,7 @@
         <v>0  (Free Rolling)</v>
       </c>
       <c r="H182" t="str">
-        <v>9</v>
+        <v>V4</v>
       </c>
     </row>
     <row r="183">
@@ -5270,7 +5270,7 @@
         <v>0  (Free Rolling)</v>
       </c>
       <c r="H189" t="str">
-        <v>V3</v>
+        <v>9</v>
       </c>
     </row>
     <row r="190">
@@ -5296,7 +5296,7 @@
         <v>0  (Free Rolling)</v>
       </c>
       <c r="H190" t="str">
-        <v>V3</v>
+        <v>9</v>
       </c>
     </row>
     <row r="191">
@@ -5322,7 +5322,7 @@
         <v>0  (Free Rolling)</v>
       </c>
       <c r="H191" t="str">
-        <v>V3</v>
+        <v>9</v>
       </c>
     </row>
     <row r="192">
@@ -5348,7 +5348,7 @@
         <v>0  (Free Rolling)</v>
       </c>
       <c r="H192" t="str">
-        <v>9</v>
+        <v>V4</v>
       </c>
     </row>
     <row r="193">
@@ -5374,7 +5374,7 @@
         <v>0  (Free Rolling)</v>
       </c>
       <c r="H193" t="str">
-        <v>9</v>
+        <v>V4</v>
       </c>
     </row>
     <row r="194">
@@ -5400,7 +5400,7 @@
         <v>0  (Free Rolling)</v>
       </c>
       <c r="H194" t="str">
-        <v>9</v>
+        <v>V4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>